<commit_message>
Detecting existing inst. names
</commit_message>
<xml_diff>
--- a/output_inst_info.xlsx
+++ b/output_inst_info.xlsx
@@ -14,17 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+  <si>
+    <t>c_inst_code</t>
+  </si>
+  <si>
+    <t>c_inst_name_hz</t>
+  </si>
   <si>
     <t>c_inst_name_code</t>
   </si>
   <si>
-    <t>c_inst_code</t>
-  </si>
-  <si>
-    <t>c_inst_name_hz</t>
-  </si>
-  <si>
     <t>c_inst_type_code</t>
   </si>
   <si>
@@ -40,16 +40,64 @@
     <t>建初寺</t>
   </si>
   <si>
+    <t>國慶寺</t>
+  </si>
+  <si>
+    <t>南巖寺</t>
+  </si>
+  <si>
+    <t>天童寺</t>
+  </si>
+  <si>
+    <t>平陽寺</t>
+  </si>
+  <si>
+    <t>天寧寺</t>
+  </si>
+  <si>
+    <t>虞山書院</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>19</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>4540</t>
   </si>
   <si>
+    <t>5402</t>
+  </si>
+  <si>
+    <t>5404</t>
+  </si>
+  <si>
+    <t>5405</t>
+  </si>
+  <si>
+    <t>7627</t>
+  </si>
+  <si>
+    <t>5398</t>
+  </si>
+  <si>
+    <t>7569</t>
+  </si>
+  <si>
+    <t>7546</t>
+  </si>
+  <si>
     <t>18417</t>
+  </si>
+  <si>
+    <t>65006</t>
   </si>
 </sst>
 </file>
@@ -407,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,25 +486,186 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>2538</v>
-      </c>
-      <c r="B2">
         <v>3920</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2">
+        <v>777</v>
+      </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>3921</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C3">
+        <v>2539</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3922</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C4">
+        <v>2540</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>3923</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C5">
+        <v>328</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>3924</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>328</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>3925</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
+      </c>
+      <c r="C7">
+        <v>2543</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>3926</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>326</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>3927</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>2350</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>